<commit_message>
commit - library list
</commit_message>
<xml_diff>
--- a/chatGPT_test/Mission/도서목록.xlsx
+++ b/chatGPT_test/Mission/도서목록.xlsx
@@ -458,187 +458,187 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>아무도 행복하지 않은 나라</t>
+          <t>이웃집 백만장자(골드 리커버 에디션)</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>김성회, 이광수, 한윤형</t>
+          <t>토머스 J. 스탠리, 윌리엄 D. 댄코/홍정희 역</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>메디치미디어</t>
+          <t>리드리드출판</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>투자의 역사는 반드시 되풀이 된다</t>
+          <t>부자 아빠 가난한 아빠 1(20주년 특별 기념판)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>정광우</t>
+          <t>로버트 기요사키/안진환 역</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>포레스트북스</t>
+          <t>민음인</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>경제 읽어주는 남자의 15분 경제 특강</t>
+          <t>마음의 지혜</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>김광석</t>
+          <t>김경일</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>더퀘스트</t>
+          <t>포레스트북스</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>부의 조건</t>
+          <t>사장학개론</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>자유지성 아카데미 17인</t>
+          <t>김승호</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>자유지성</t>
+          <t>스노우폭스북스</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>설민석의 한국사 대모험 25</t>
+          <t>하늘과 바람과 별과 인간</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>설민석, 스토리박스/정현희 그림/강석화 감수</t>
+          <t>김상욱</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>단꿈아이</t>
+          <t>바다출판사</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>역행자(확장판)</t>
+          <t>알아차림에 대한 알아차림</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>자청</t>
+          <t>루퍼트 스파이라</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>웅진지식하우스</t>
+          <t>퍼블리온</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>메리골드 마음 세탁소</t>
+          <t>이미 늦었다고 생각하는 당신을 위한 김미경의 마흔 수업</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>윤정은</t>
+          <t>김미경</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>북로망스</t>
+          <t>어웨이크북스</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>건강과 다이어트를 동시에 잡는 7대 3의 법칙 채소·과일식</t>
+          <t>메리골드 마음 세탁소</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>조승우</t>
+          <t>윤정은</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>바이북스</t>
+          <t>북로망스</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>모성</t>
+          <t>백만장자 메신저</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>미나토 가나에(湊かなえ)</t>
+          <t>브렌든 버처드/위선주 역</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>리드리드출판</t>
+          <t>리더스북</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>하늘과 바람과 별과 인간</t>
+          <t>실전 매수매도 기법</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>김상욱</t>
+          <t>김영옥(데이짱)</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>바다출판사</t>
+          <t>이레미디어</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>당신의 남자를 죽여드립니다</t>
+          <t>부의 조건</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>엘 코시마노</t>
+          <t>자유지성 아카데미 17인</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>인플루엔셜</t>
+          <t>자유지성</t>
         </is>
       </c>
     </row>
@@ -662,34 +662,34 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>바다가 들리는 편의점</t>
+          <t>나의 돈 많은 고등학교 친구</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>마치다 소노코/황국영 역</t>
+          <t>송희구</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>모모</t>
+          <t>서삼독</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>만일 내가 인생을 다시 산다면(30만 부 기념 리커버 에디션)</t>
+          <t>2023 제14회 젊은작가상 수상작품집</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>김혜남</t>
+          <t>이미상, 김멜라, 성혜령, 이서수, 정선임</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>메이븐</t>
+          <t>문학동네</t>
         </is>
       </c>
     </row>

</xml_diff>